<commit_message>
2nd Sept Array + String
</commit_message>
<xml_diff>
--- a/Practice Sheet.xlsx
+++ b/Practice Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axdit\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B00E16-6093-4042-A32B-59B16306CF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F29304-CDB8-4847-BC40-328A9457B1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>S. No</t>
   </si>
@@ -51,30 +51,42 @@
     <t>Solution Link</t>
   </si>
   <si>
-    <t>Editorial</t>
-  </si>
-  <si>
     <t>Array</t>
   </si>
   <si>
     <t>https://leetcode.com/problems/3sum/description/</t>
   </si>
   <si>
+    <t>https://leetcode.com/problems/longest-substring-without-repeating-characters/description/</t>
+  </si>
+  <si>
     <t>https://leetcode.com/problems/two-sum/description/</t>
   </si>
   <si>
     <t>Two Sum</t>
   </si>
   <si>
+    <t> String to Integer (atoi)</t>
+  </si>
+  <si>
     <t>Container With Most Water</t>
   </si>
   <si>
+    <t> Integer to Roman</t>
+  </si>
+  <si>
+    <t>Roman to Integer</t>
+  </si>
+  <si>
     <t> 3Sum</t>
   </si>
   <si>
     <t>3Sum Closest</t>
   </si>
   <si>
+    <t> Implement strStr()</t>
+  </si>
+  <si>
     <t>Sept</t>
   </si>
   <si>
@@ -112,6 +124,39 @@
   </si>
   <si>
     <t>Two-pointer, Dynamic Prgramming, Monotinic Stack</t>
+  </si>
+  <si>
+    <t>Longest Substring W/O Repeating Characters</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Sliding Window, Hash Table</t>
+  </si>
+  <si>
+    <t>Rotate Image</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotate-image/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-the-index-of-the-first-occurrence-in-a-string/description/</t>
+  </si>
+  <si>
+    <t>Two-Pointer, String Matching</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/string-to-integer-atoi/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/roman-to-integer/description/</t>
+  </si>
+  <si>
+    <t>Logic</t>
   </si>
 </sst>
 </file>
@@ -525,7 +570,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.1796875" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -553,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>3</v>
@@ -570,22 +615,20 @@
       <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>8</v>
-      </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
@@ -597,7 +640,7 @@
         <v>45536</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="1"/>
@@ -607,25 +650,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="G3" s="4">
         <v>45536</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="1"/>
@@ -635,25 +678,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G4" s="4">
         <v>45536</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="1"/>
@@ -663,25 +706,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G5" s="4">
         <v>45536</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="1"/>
@@ -691,98 +734,194 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="G6" s="4">
         <v>45536</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="1"/>
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="4">
+        <v>45537</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="I7" s="8"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="1"/>
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="4">
+        <v>45537</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="I8" s="8"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="4">
+        <v>45537</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="4">
+        <v>45537</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="4">
+        <v>45537</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="1"/>
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4">
+        <v>45537</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="I12" s="8"/>
       <c r="J12" s="1"/>
     </row>

</xml_diff>

<commit_message>
4th Sept Linked List
</commit_message>
<xml_diff>
--- a/Practice Sheet.xlsx
+++ b/Practice Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axdit\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC781B9-7BF4-4A08-8A17-FA86E5B64009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767CFFA0-921A-4B78-B4BD-64ED2A297285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-220" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15230" yWindow="-21600" windowWidth="17130" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="69">
   <si>
     <t>S. No</t>
   </si>
@@ -208,13 +208,37 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/group-anagrams/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/copy-list-with-random-pointer/description/</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>Copy List with Random Pointer</t>
+  </si>
+  <si>
+    <t>Add Two Numbers</t>
+  </si>
+  <si>
+    <t>Recursion, Math</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-two-numbers/description/</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-sorted-lists/description/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,27 +263,11 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <u/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -308,23 +316,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -609,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.1796875" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -619,8 +627,8 @@
     <col min="2" max="2" width="9" style="3" customWidth="1"/>
     <col min="3" max="3" width="40" style="3" customWidth="1"/>
     <col min="4" max="4" width="11.54296875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="37.26953125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="47.1796875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="35.7265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="51" style="3" customWidth="1"/>
     <col min="7" max="8" width="10.1796875" style="3"/>
     <col min="9" max="9" width="16.36328125" style="3" customWidth="1"/>
     <col min="10" max="10" width="17.7265625" style="3" customWidth="1"/>
@@ -628,31 +636,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -675,16 +683,16 @@
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="2">
         <v>45536</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="4"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -703,16 +711,16 @@
       <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="2">
         <v>45536</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="4"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -731,16 +739,16 @@
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G4" s="2">
         <v>45536</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="4"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -759,16 +767,16 @@
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="2">
         <v>45536</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="4"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -787,16 +795,16 @@
       <c r="E6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="2">
         <v>45536</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="4"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -812,7 +820,7 @@
       <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -821,10 +829,10 @@
       <c r="G7" s="2">
         <v>45537</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="4"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -843,16 +851,16 @@
       <c r="E8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G8" s="2">
         <v>45537</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="4"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -868,16 +876,16 @@
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G9" s="2">
         <v>45537</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I9" s="1"/>
@@ -899,13 +907,13 @@
       <c r="E10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G10" s="2">
         <v>45537</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I10" s="1"/>
@@ -927,13 +935,13 @@
       <c r="E11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>47</v>
       </c>
       <c r="G11" s="2">
         <v>45538</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I11" s="1"/>
@@ -955,16 +963,16 @@
       <c r="E12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G12" s="2">
         <v>45537</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="4"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -983,7 +991,7 @@
       <c r="E13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="2">
@@ -992,7 +1000,7 @@
       <c r="H13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1008,10 +1016,10 @@
       <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G14" s="2">
@@ -1020,7 +1028,7 @@
       <c r="H14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="4"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1036,10 +1044,10 @@
       <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>53</v>
       </c>
       <c r="G15" s="2">
@@ -1064,10 +1072,10 @@
       <c r="D16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="8" t="s">
         <v>56</v>
       </c>
       <c r="G16" s="2">
@@ -1076,7 +1084,7 @@
       <c r="H16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="4"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1092,10 +1100,10 @@
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G17" s="2">
@@ -1132,33 +1140,96 @@
       <c r="H18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="9"/>
+      <c r="I18" s="7"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="2">
+        <v>45539</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="2">
+        <v>45539</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="2">
+        <v>45539</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="2"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1346,6 +1417,10 @@
       <c r="J38" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F20" r:id="rId1" xr:uid="{7DF8B1A5-BA32-4A02-ACF5-5F55C1C4BBE4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding JavaScript DSA Problems
</commit_message>
<xml_diff>
--- a/Practice Sheet.xlsx
+++ b/Practice Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axdit\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07D8E0F-F60E-4561-A9FD-6E0A68B58377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A439D1-D222-49D7-BE72-832B6701CB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5280" yWindow="-18617" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5443" yWindow="-18617" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="81">
   <si>
     <t>S. No</t>
   </si>
@@ -242,6 +242,27 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/reverse-linked-list/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-number/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-common-prefix/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-anagram/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-common-prefix/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-strings-alternately/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/length-of-last-word/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-characters-by-frequency/description/</t>
   </si>
 </sst>
 </file>
@@ -677,8 +698,8 @@
   </sheetPr>
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.4"/>
@@ -1345,9 +1366,21 @@
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="5"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="4"/>
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="7">
+        <v>45556</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
@@ -1357,9 +1390,15 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="4"/>
+      <c r="F25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="7">
+        <v>45556</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
@@ -1369,9 +1408,15 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="4"/>
+      <c r="F26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="7">
+        <v>45556</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
@@ -1381,9 +1426,15 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="7">
+        <v>45556</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
     </row>
@@ -1393,9 +1444,15 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="4"/>
+      <c r="F28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="7">
+        <v>45556</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
@@ -1405,9 +1462,15 @@
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="4"/>
+      <c r="F29" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G29" s="7">
+        <v>45556</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
@@ -1417,9 +1480,15 @@
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="4"/>
+      <c r="F30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="7">
+        <v>45556</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
@@ -1429,9 +1498,15 @@
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="7">
+        <v>45556</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
@@ -1441,9 +1516,15 @@
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="4"/>
+      <c r="F32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G32" s="7">
+        <v>45556</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>

</xml_diff>